<commit_message>
Added form states, timeseries and other queries
</commit_message>
<xml_diff>
--- a/appmodel/app-model.xlsx
+++ b/appmodel/app-model.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navendusinha/PycharmProjects/neoWebUI/appmodel/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C853DDDA-9064-0847-BE77-A475474C3741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ABE4F2-D591-3244-B276-6DB36DCFA08D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4820" yWindow="720" windowWidth="28040" windowHeight="17440" activeTab="2" xr2:uid="{B230B229-1191-BA4F-B757-C9FE5A580652}"/>
+    <workbookView xWindow="3660" yWindow="1200" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{B230B229-1191-BA4F-B757-C9FE5A580652}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="47">
   <si>
     <t>Appname</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Doe</t>
   </si>
   <si>
-    <t>UserID</t>
-  </si>
-  <si>
     <t>email</t>
   </si>
   <si>
@@ -142,9 +139,6 @@
     <t>TestAppDB</t>
   </si>
   <si>
-    <t>DatabaseTables</t>
-  </si>
-  <si>
     <t>COL#</t>
   </si>
   <si>
@@ -169,6 +163,9 @@
     <t>COL4</t>
   </si>
   <si>
+    <t>authorization</t>
+  </si>
+  <si>
     <t>signin</t>
   </si>
   <si>
@@ -188,13 +185,31 @@
   </si>
   <si>
     <t>distinct('License')</t>
+  </si>
+  <si>
+    <t>API Signature</t>
+  </si>
+  <si>
+    <t>find({'</t>
+  </si>
+  <si>
+    <t>signup</t>
+  </si>
+  <si>
+    <t>password</t>
+  </si>
+  <si>
+    <t>TableName</t>
+  </si>
+  <si>
+    <t>userid</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -212,6 +227,14 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -351,7 +374,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
@@ -366,10 +388,11 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -698,7 +721,7 @@
         <v>0</v>
       </c>
       <c r="C1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.2">
@@ -706,7 +729,7 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -716,10 +739,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DEC91076-B794-D24C-81D3-BD11A24F9ACB}">
-  <dimension ref="B1:E8"/>
+  <dimension ref="B1:E11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -729,22 +752,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B1" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="E1" t="s">
-        <v>23</v>
+      <c r="E1" s="12" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -758,7 +781,7 @@
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -772,78 +795,122 @@
     </row>
     <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" t="s">
-        <v>35</v>
+        <v>43</v>
       </c>
       <c r="C4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="5" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B5" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>14</v>
+        <v>44</v>
       </c>
       <c r="D5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" t="s">
-        <v>15</v>
+        <v>44</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" t="s">
         <v>13</v>
-      </c>
-      <c r="C6" t="s">
-        <v>16</v>
       </c>
       <c r="D6" t="s">
         <v>6</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D7" t="s">
         <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>6</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
         <v>20</v>
       </c>
-      <c r="D8" t="s">
+      <c r="E9" t="s">
         <v>21</v>
       </c>
-      <c r="E8" t="s">
-        <v>22</v>
+    </row>
+    <row r="10" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" t="s">
+        <v>10</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B11" t="s">
+        <v>34</v>
+      </c>
+      <c r="C11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D11" t="s">
+        <v>44</v>
+      </c>
+      <c r="E11" t="s">
+        <v>44</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="E4" r:id="rId1" xr:uid="{5D92B118-9E6F-3A4F-BD5E-609150A1352B}"/>
+    <hyperlink ref="E5" r:id="rId1" display="johndoe@email.com" xr:uid="{5D92B118-9E6F-3A4F-BD5E-609150A1352B}"/>
+    <hyperlink ref="E10" r:id="rId2" xr:uid="{D65AD12B-2157-B548-B8F7-6D3CD4F58E1D}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{FE7300D1-33D2-3248-9DB9-F081C6B15198}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -851,34 +918,46 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25CEE5AD-978B-C346-AB0D-436CE01C7E14}">
-  <dimension ref="B1:D2"/>
+  <dimension ref="B1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="31.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D1" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" t="s">
         <v>39</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
-      <c r="B2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" t="s">
-        <v>41</v>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>
@@ -888,45 +967,61 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B0635B-1A6B-4E4D-B464-016C4F031864}">
-  <dimension ref="B1:C3"/>
+  <dimension ref="B1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="20" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="4" max="4" width="14.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="2:3" x14ac:dyDescent="0.2">
+        <v>2</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="12" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B2" t="str" cm="1">
-        <f t="array" ref="B2:B3">_xlfn.UNIQUE(Forms!B2:B8)</f>
-        <v>signin</v>
+        <f t="array" ref="B2:B4">_xlfn.UNIQUE(Forms!B2:B10)</f>
+        <v>signup</v>
       </c>
       <c r="C2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4" x14ac:dyDescent="0.2">
       <c r="B3" t="str">
         <v>parkingreq</v>
       </c>
       <c r="C3" t="s">
-        <v>37</v>
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B4" t="str">
+        <v>signin</v>
+      </c>
+      <c r="C4" t="s">
+        <v>33</v>
+      </c>
+      <c r="D4" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
@@ -942,34 +1037,34 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C1" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E1" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="F1" s="10" t="s">
         <v>32</v>
-      </c>
-      <c r="E1" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" s="12" t="s">
+      <c r="C2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="13"/>
+      <c r="F2" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="E2" s="12"/>
-      <c r="F2" s="8" t="s">
-        <v>30</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
@@ -977,218 +1072,178 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="C3" s="4"/>
-      <c r="F3" s="5"/>
+      <c r="C3" s="3"/>
+      <c r="F3" s="4"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <f t="shared" ref="A4:A24" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="5"/>
+      <c r="C4" s="3"/>
+      <c r="F4" s="4"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="F5" s="5"/>
+      <c r="C5" s="3"/>
+      <c r="F5" s="4"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="5"/>
+      <c r="C6" s="3"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="5"/>
+      <c r="C7" s="3"/>
+      <c r="F7" s="4"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="5"/>
+      <c r="C8" s="3"/>
+      <c r="F8" s="4"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C9" s="4"/>
-      <c r="D9" s="3"/>
-      <c r="E9" s="3"/>
-      <c r="F9" s="5"/>
+      <c r="C9" s="3"/>
+      <c r="F9" s="4"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C10" s="4"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="5"/>
+      <c r="C10" s="3"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="C11" s="4"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="5"/>
+      <c r="C11" s="3"/>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="C12" s="4"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="5"/>
+      <c r="C12" s="3"/>
+      <c r="F12" s="4"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="C13" s="4"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="3"/>
-      <c r="F13" s="5"/>
+      <c r="C13" s="3"/>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="C14" s="4"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="5"/>
+      <c r="C14" s="3"/>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="C15" s="4"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" s="5"/>
+      <c r="C15" s="3"/>
+      <c r="F15" s="4"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="C16" s="4"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="5"/>
+      <c r="C16" s="3"/>
+      <c r="F16" s="4"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" s="5"/>
+      <c r="C17" s="3"/>
+      <c r="F17" s="4"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="5"/>
+      <c r="C18" s="3"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C19" s="4"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
-      <c r="F19" s="5"/>
+      <c r="C19" s="3"/>
+      <c r="F19" s="4"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="C20" s="4"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="5"/>
+      <c r="C20" s="3"/>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="C21" s="4"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
-      <c r="F21" s="5"/>
+      <c r="C21" s="3"/>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="C22" s="4"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="5"/>
+      <c r="C22" s="3"/>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="C23" s="4"/>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" s="5"/>
+      <c r="C23" s="3"/>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="C24" s="6"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="7"/>
-      <c r="F24" s="8"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>